<commit_message>
logic file final update
</commit_message>
<xml_diff>
--- a/logic-file/manager-logic.xlsx
+++ b/logic-file/manager-logic.xlsx
@@ -1,25 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\SkyFitness\logic-file\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9F624B-E4AB-469E-AC4A-0E90EBC817EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2579" yWindow="2579" windowWidth="18851" windowHeight="9766" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>Lương cơ bản</t>
+  </si>
+  <si>
+    <t>Tháng cao điểm (3-12)</t>
+  </si>
+  <si>
+    <t>Tháng thấp điểm (1-2)</t>
+  </si>
+  <si>
+    <t>% Doanh số</t>
+  </si>
+  <si>
+    <t>% lương CB</t>
+  </si>
+  <si>
+    <t>&lt;300</t>
+  </si>
+  <si>
+    <t>300-350</t>
+  </si>
+  <si>
+    <t>250-300</t>
+  </si>
+  <si>
+    <t>&lt;250</t>
+  </si>
+  <si>
+    <t>&gt;500</t>
+  </si>
+  <si>
+    <t>350-400</t>
+  </si>
+  <si>
+    <t>400-450</t>
+  </si>
+  <si>
+    <t>450-500</t>
+  </si>
+  <si>
+    <t>Tháng</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +93,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +115,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +422,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>11000000</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>